<commit_message>
1st tier button clicks are now properly routed. click changes view state value in model, which then emits value to view
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\OneDrive - Kansas State University\2019 - Fall\CIS 598 - CompSciProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="13_ncr:1_{C9FB6E23-25C8-4249-BD92-3E0286B9E232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8CECB30D-DFF7-41EB-A718-14F513CE61DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC3582F-FB8B-49DE-8A08-C5BB911A6211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
+    <workbookView xWindow="4290" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t>Delta</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>5:50PM</t>
+  </si>
+  <si>
+    <t>Setting up other buttons; rerouting signals to correctly change model and have view react to model parameter changes</t>
   </si>
 </sst>
 </file>
@@ -638,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G43"/>
+  <dimension ref="A3:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,6 +1136,17 @@
         <v>79</v>
       </c>
     </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43789</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
entered logbook entry for last commit
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC3582F-FB8B-49DE-8A08-C5BB911A6211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C826A6DF-3D83-4408-AEE6-505DCA8B3674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t>Delta</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Setting up other buttons; rerouting signals to correctly change model and have view react to model parameter changes</t>
+  </si>
+  <si>
+    <t>5:10PM</t>
   </si>
 </sst>
 </file>
@@ -644,7 +647,7 @@
   <dimension ref="A3:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,6 +1146,15 @@
       <c r="B45" t="s">
         <v>27</v>
       </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>80</v>
+      </c>
       <c r="F45" t="s">
         <v>81</v>
       </c>

</xml_diff>

<commit_message>
can add new clients now. need to create dialog popup to state that new client has been created
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C826A6DF-3D83-4408-AEE6-505DCA8B3674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D578639-4155-4800-BDE4-CE5EF0118BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>Delta</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>5:10PM</t>
+  </si>
+  <si>
+    <t>6:00PM</t>
+  </si>
+  <si>
+    <t>Building newClient view and setting signals/buttons to show view upon clicking new client button</t>
   </si>
 </sst>
 </file>
@@ -644,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G45"/>
+  <dimension ref="A3:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,6 +1165,20 @@
         <v>81</v>
       </c>
     </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46">
+        <v>50</v>
+      </c>
+      <c r="F46" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated logbook to reflect last commit
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D578639-4155-4800-BDE4-CE5EF0118BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6B510E-45D5-419B-A2E8-35C5CCC6CA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>Delta</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Building newClient view and setting signals/buttons to show view upon clicking new client button</t>
+  </si>
+  <si>
+    <t>7:00PM</t>
+  </si>
+  <si>
+    <t>Connected new client click action with insert statement into sql db; db now creates new clients and doesn't crash when the unique name constraint is violated. Need to put popup dialog after new client button click to show user the client has succcessfuly been added or not</t>
   </si>
 </sst>
 </file>
@@ -650,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G46"/>
+  <dimension ref="A3:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,6 +1185,20 @@
         <v>84</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47">
+        <v>60</v>
+      </c>
+      <c r="F47" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added signal to modify user-given text in text boxes depending on call to db being a success or fail
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6B510E-45D5-419B-A2E8-35C5CCC6CA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAC70EF-F0BB-4743-9B32-1FBA836B10E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="2715" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
   <si>
     <t>Delta</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Connected new client click action with insert statement into sql db; db now creates new clients and doesn't crash when the unique name constraint is violated. Need to put popup dialog after new client button click to show user the client has succcessfuly been added or not</t>
+  </si>
+  <si>
+    <t>Setting up generic messageBox to show confirmation or error msg to user</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G47"/>
+  <dimension ref="A3:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,6 +1202,23 @@
         <v>86</v>
       </c>
     </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>43791</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49">
+        <v>90</v>
+      </c>
+      <c r="F49" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
client list now shows in listView
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAC70EF-F0BB-4743-9B32-1FBA836B10E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E746BFC-A60F-4E6F-B1F9-77CE9CE1F38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
   <si>
     <t>Delta</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Setting up generic messageBox to show confirmation or error msg to user</t>
+  </si>
+  <si>
+    <t>1:30PM</t>
   </si>
 </sst>
 </file>
@@ -659,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G49"/>
+  <dimension ref="A3:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,6 +1222,14 @@
         <v>87</v>
       </c>
     </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>43795</v>
+      </c>
+      <c r="B51" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
need to now setup the changing of client info with the newly placed information by the user
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E746BFC-A60F-4E6F-B1F9-77CE9CE1F38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D72EAC-A01F-4A3B-956C-7ECD8959605D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
   <si>
     <t>Delta</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>1:30PM</t>
+  </si>
+  <si>
+    <t>Getting the Search/Edit Cllient info page to work correctly</t>
+  </si>
+  <si>
+    <t>Everything except db call to change info is setup. Display is proper with user interaction.</t>
   </si>
 </sst>
 </file>
@@ -665,7 +671,7 @@
   <dimension ref="A3:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1211,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43791</v>
       </c>
@@ -1222,12 +1228,27 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43795</v>
       </c>
       <c r="B51" t="s">
         <v>88</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51">
+        <v>30</v>
+      </c>
+      <c r="E51">
+        <v>230</v>
+      </c>
+      <c r="F51" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit client info now completed. New tables have been defined. Starting on new product page
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D72EAC-A01F-4A3B-956C-7ECD8959605D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D32DA5F-6220-4ECD-8261-90881807A559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
   <si>
     <t>Delta</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>Everything except db call to change info is setup. Display is proper with user interaction.</t>
+  </si>
+  <si>
+    <t>10:50AM</t>
   </si>
 </sst>
 </file>
@@ -668,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G51"/>
+  <dimension ref="A3:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,6 +1254,14 @@
         <v>90</v>
       </c>
     </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>43796</v>
+      </c>
+      <c r="B53" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
newProduct logic finished => can successfully add new products to db.
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D32DA5F-6220-4ECD-8261-90881807A559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21134E2D-DFDA-4E5D-9C01-3829939D86D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="95">
   <si>
     <t>Delta</t>
   </si>
@@ -301,6 +301,15 @@
   </si>
   <si>
     <t>10:50AM</t>
+  </si>
+  <si>
+    <t>12:40PM</t>
+  </si>
+  <si>
+    <t>Finalizing searchEditClients page/creating and adding newProduct page</t>
+  </si>
+  <si>
+    <t>newProduct page now just needs the code to add prods to db.</t>
   </si>
 </sst>
 </file>
@@ -671,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G53"/>
+  <dimension ref="A3:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,6 +1270,26 @@
       <c r="B53" t="s">
         <v>91</v>
       </c>
+      <c r="C53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53" t="s">
+        <v>93</v>
+      </c>
+      <c r="G53" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added line in logbook
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21134E2D-DFDA-4E5D-9C01-3829939D86D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFB52C7-80C9-4791-8C85-4797EADEE9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
   <si>
     <t>Delta</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>newProduct page now just needs the code to add prods to db.</t>
+  </si>
+  <si>
+    <t>Finish newProd page ui and code; start on newOrder page and code</t>
+  </si>
+  <si>
+    <t>currently finished newProd page and code; majority of fields in newOrder page display correctly now. Next is to code the adding of products to the current order and successfully add the order to the db</t>
   </si>
 </sst>
 </file>
@@ -683,7 +689,7 @@
   <dimension ref="A3:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,6 +1296,21 @@
       <c r="B54" t="s">
         <v>74</v>
       </c>
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54">
+        <v>20</v>
+      </c>
+      <c r="E54">
+        <v>170</v>
+      </c>
+      <c r="F54" t="s">
+        <v>95</v>
+      </c>
+      <c r="G54" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Coded SQL DB functions for inserting orders and their products. Coded GUI response to changing the amount per product so that the total value appears
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFB52C7-80C9-4791-8C85-4797EADEE9B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5427BC-D918-4A40-B5A6-0D2420A152B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
+    <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
   <si>
     <t>Delta</t>
   </si>
@@ -111,9 +111,6 @@
     <t>3:30PM</t>
   </si>
   <si>
-    <t>60 mins</t>
-  </si>
-  <si>
     <t xml:space="preserve">Assessing libraries and licenses needed </t>
   </si>
   <si>
@@ -316,6 +313,39 @@
   </si>
   <si>
     <t>currently finished newProd page and code; majority of fields in newOrder page display correctly now. Next is to code the adding of products to the current order and successfully add the order to the db</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>~180</t>
+  </si>
+  <si>
+    <t>Activity Summary</t>
+  </si>
+  <si>
+    <t>Research Reading</t>
+  </si>
+  <si>
+    <t>Defining Project Idea</t>
+  </si>
+  <si>
+    <t>Code/Debug</t>
+  </si>
+  <si>
+    <t>Finished newOrder GUI functionality; Need to implement adding data to DB now</t>
+  </si>
+  <si>
+    <t>12:58PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generating Code </t>
+  </si>
+  <si>
+    <t>1:28PM</t>
+  </si>
+  <si>
+    <t>Added functions for DB editing; debugged GUI issues (e.g. user could press "add product to order" button when no products were available to add, leading to crash)</t>
   </si>
 </sst>
 </file>
@@ -686,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:G54"/>
+  <dimension ref="A3:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,20 +729,20 @@
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
     <col min="6" max="6" width="68" customWidth="1"/>
-    <col min="7" max="7" width="118.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="111" customWidth="1"/>
+    <col min="8" max="8" width="90.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>101419</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -732,10 +762,13 @@
         <v>5</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43705</v>
       </c>
@@ -752,13 +785,16 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" t="s">
         <v>7</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43705</v>
       </c>
@@ -775,13 +811,16 @@
         <v>16</v>
       </c>
       <c r="F14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43726</v>
       </c>
@@ -795,13 +834,16 @@
         <v>120</v>
       </c>
       <c r="F16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" t="s">
         <v>19</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -811,14 +853,17 @@
       <c r="E17">
         <v>60</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43745</v>
       </c>
@@ -828,14 +873,17 @@
       <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" t="s">
         <v>28</v>
       </c>
-      <c r="F18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43747</v>
       </c>
@@ -843,21 +891,24 @@
         <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19">
         <v>60</v>
       </c>
       <c r="F19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" t="s">
         <v>30</v>
       </c>
-      <c r="G19" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
@@ -866,61 +917,70 @@
         <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>43749</v>
       </c>
       <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
         <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
       </c>
       <c r="E21">
         <v>80</v>
       </c>
       <c r="F21" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>43752</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22">
         <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23">
         <v>30</v>
       </c>
-      <c r="F23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>43756</v>
       </c>
@@ -928,7 +988,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -936,22 +996,22 @@
       <c r="E24">
         <v>140</v>
       </c>
-      <c r="F24" t="s">
-        <v>41</v>
-      </c>
       <c r="G24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>43769</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -959,14 +1019,14 @@
       <c r="E26">
         <v>110</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" t="s">
         <v>45</v>
       </c>
-      <c r="G26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>43770</v>
       </c>
@@ -974,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -982,22 +1042,22 @@
       <c r="E28">
         <v>140</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" t="s">
         <v>47</v>
       </c>
-      <c r="G28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43773</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30">
         <v>40</v>
@@ -1005,22 +1065,22 @@
       <c r="E30">
         <v>190</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" t="s">
         <v>50</v>
       </c>
-      <c r="G30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43776</v>
       </c>
       <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
         <v>53</v>
-      </c>
-      <c r="C32" t="s">
-        <v>54</v>
       </c>
       <c r="D32">
         <v>15</v>
@@ -1028,31 +1088,31 @@
       <c r="E32">
         <v>120</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
+        <v>54</v>
+      </c>
+      <c r="H32" t="s">
         <v>55</v>
       </c>
-      <c r="G32" t="s">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>57</v>
-      </c>
-      <c r="C33" t="s">
-        <v>58</v>
       </c>
       <c r="E33">
         <v>30</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" t="s">
         <v>59</v>
       </c>
-      <c r="G33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43777</v>
       </c>
@@ -1060,7 +1120,7 @@
         <v>26</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1068,16 +1128,16 @@
       <c r="E35">
         <v>50</v>
       </c>
-      <c r="F35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1085,22 +1145,22 @@
       <c r="E36">
         <v>90</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" t="s">
         <v>65</v>
       </c>
-      <c r="G36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43782</v>
       </c>
       <c r="B38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
         <v>67</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
       </c>
       <c r="D38">
         <v>30</v>
@@ -1108,22 +1168,22 @@
       <c r="E38">
         <v>90</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" t="s">
         <v>69</v>
       </c>
-      <c r="G38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43784</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1131,22 +1191,22 @@
       <c r="E40">
         <v>85</v>
       </c>
-      <c r="F40" t="s">
-        <v>69</v>
-      </c>
       <c r="G40" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43788</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D42">
         <v>20</v>
@@ -1154,19 +1214,19 @@
       <c r="E42">
         <v>130</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" t="s">
         <v>75</v>
       </c>
-      <c r="G42" t="s">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="C43" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D43">
         <v>10</v>
@@ -1174,14 +1234,14 @@
       <c r="E43">
         <v>70</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43" t="s">
         <v>78</v>
       </c>
-      <c r="G43" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43789</v>
       </c>
@@ -1189,7 +1249,7 @@
         <v>27</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D45">
         <v>20</v>
@@ -1197,64 +1257,64 @@
       <c r="E45">
         <v>80</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>82</v>
-      </c>
-      <c r="C46" t="s">
-        <v>83</v>
       </c>
       <c r="E46">
         <v>50</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" t="s">
-        <v>85</v>
       </c>
       <c r="E47">
         <v>60</v>
       </c>
-      <c r="F47" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43791</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E49">
         <v>90</v>
       </c>
-      <c r="F49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>43795</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D51">
         <v>30</v>
@@ -1262,22 +1322,22 @@
       <c r="E51">
         <v>230</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
+        <v>88</v>
+      </c>
+      <c r="H51" t="s">
         <v>89</v>
       </c>
-      <c r="G51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43796</v>
       </c>
       <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" t="s">
         <v>91</v>
-      </c>
-      <c r="C53" t="s">
-        <v>92</v>
       </c>
       <c r="D53">
         <v>10</v>
@@ -1285,19 +1345,19 @@
       <c r="E53">
         <v>100</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
+        <v>92</v>
+      </c>
+      <c r="H53" t="s">
         <v>93</v>
       </c>
-      <c r="G53" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D54">
         <v>20</v>
@@ -1305,11 +1365,51 @@
       <c r="E54">
         <v>170</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
+        <v>94</v>
+      </c>
+      <c r="H54" t="s">
         <v>95</v>
       </c>
-      <c r="G54" t="s">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>43808</v>
+      </c>
+      <c r="B56" t="s">
         <v>96</v>
+      </c>
+      <c r="C56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" t="s">
+        <v>97</v>
+      </c>
+      <c r="F56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>43809</v>
+      </c>
+      <c r="B58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58">
+        <v>30</v>
+      </c>
+      <c r="F58" t="s">
+        <v>104</v>
+      </c>
+      <c r="G58" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formatted the order confirmation dialog box
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5427BC-D918-4A40-B5A6-0D2420A152B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497E089B-7AC8-4A73-A375-C11F231388C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="110">
   <si>
     <t>Delta</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>Added functions for DB editing; debugged GUI issues (e.g. user could press "add product to order" button when no products were available to add, leading to crash)</t>
+  </si>
+  <si>
+    <t>1:42PM</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t>Debugging the New Order GUI response to changing product amounts while in-order list</t>
   </si>
 </sst>
 </file>
@@ -716,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H58"/>
+  <dimension ref="A3:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,6 +1421,23 @@
         <v>106</v>
       </c>
     </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>108</v>
+      </c>
+      <c r="G59" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
debugged data generation from new order page
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497E089B-7AC8-4A73-A375-C11F231388C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC2B1E-3A9F-487B-A69B-D67F867ED61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
   <si>
     <t>Delta</t>
   </si>
@@ -355,6 +355,27 @@
   </si>
   <si>
     <t>Debugging the New Order GUI response to changing product amounts while in-order list</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Formatting the new order confirmation dialog pop-up box</t>
+  </si>
+  <si>
+    <t>Get total value amounts from all products in order and add to order</t>
+  </si>
+  <si>
+    <t>2:53PM</t>
+  </si>
+  <si>
+    <t>Orders now get added to DB. Now need to add prods too</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Debugging sql inserts and queries for newOrder and products in new order</t>
   </si>
 </sst>
 </file>
@@ -725,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H59"/>
+  <dimension ref="A3:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +758,7 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="68" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
     <col min="7" max="7" width="111" customWidth="1"/>
     <col min="8" max="8" width="90.42578125" customWidth="1"/>
   </cols>
@@ -1438,6 +1459,54 @@
         <v>109</v>
       </c>
     </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="4">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="C60" s="4">
+        <v>7.8472222222222221E-2</v>
+      </c>
+      <c r="E60">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>110</v>
+      </c>
+      <c r="G60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="4">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>113</v>
+      </c>
+      <c r="E61">
+        <v>36</v>
+      </c>
+      <c r="F61" t="s">
+        <v>110</v>
+      </c>
+      <c r="G61" t="s">
+        <v>112</v>
+      </c>
+      <c r="H61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62" t="s">
+        <v>115</v>
+      </c>
+      <c r="G62" t="s">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
successfully adds a new order and its products to the db. now to create invoices from the orders
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC2B1E-3A9F-487B-A69B-D67F867ED61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1868BA4C-85D5-4E22-BDFA-699758B19E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
   <si>
     <t>Delta</t>
   </si>
@@ -376,6 +376,18 @@
   </si>
   <si>
     <t>Debugging sql inserts and queries for newOrder and products in new order</t>
+  </si>
+  <si>
+    <t>Debugged inserts into Orders table in db. All good now</t>
+  </si>
+  <si>
+    <t>3:40PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code </t>
+  </si>
+  <si>
+    <t>Adding Products to OrderItems table from given products in order</t>
   </si>
 </sst>
 </file>
@@ -746,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H62"/>
+  <dimension ref="A3:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,11 +1512,31 @@
       <c r="B62" t="s">
         <v>113</v>
       </c>
+      <c r="C62" s="4">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="E62">
+        <v>47</v>
+      </c>
       <c r="F62" t="s">
         <v>115</v>
       </c>
       <c r="G62" t="s">
         <v>116</v>
+      </c>
+      <c r="H62" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>118</v>
+      </c>
+      <c r="F63" t="s">
+        <v>119</v>
+      </c>
+      <c r="G63" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Successfully creates SQL tables for invoices
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1868BA4C-85D5-4E22-BDFA-699758B19E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11BE0B3-010C-4401-B5AB-FB248249DC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
   <si>
     <t>Delta</t>
   </si>
@@ -384,10 +384,19 @@
     <t>3:40PM</t>
   </si>
   <si>
-    <t xml:space="preserve">Code </t>
-  </si>
-  <si>
     <t>Adding Products to OrderItems table from given products in order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code/Debug </t>
+  </si>
+  <si>
+    <t>4:18PM</t>
+  </si>
+  <si>
+    <t>Now that adding orders to db is complete, now to add invoices</t>
+  </si>
+  <si>
+    <t>Generate Invoices GUI page and functionality start</t>
   </si>
 </sst>
 </file>
@@ -758,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H63"/>
+  <dimension ref="A3:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,11 +1541,28 @@
       <c r="B63" t="s">
         <v>118</v>
       </c>
+      <c r="C63" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="F63" t="s">
+        <v>120</v>
+      </c>
+      <c r="G63" t="s">
         <v>119</v>
       </c>
-      <c r="G63" t="s">
-        <v>120</v>
+      <c r="H63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>121</v>
+      </c>
+      <c r="F64" t="s">
+        <v>110</v>
+      </c>
+      <c r="G64" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Invoice GUI now correctly displays. Onto connecting the buttons and settings for it
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11BE0B3-010C-4401-B5AB-FB248249DC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63486BA-ECB5-497C-BD59-8B9909EFB79D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="130">
   <si>
     <t>Delta</t>
   </si>
@@ -397,6 +397,24 @@
   </si>
   <si>
     <t>Generate Invoices GUI page and functionality start</t>
+  </si>
+  <si>
+    <t>4:34PM</t>
+  </si>
+  <si>
+    <t>Debugged as well</t>
+  </si>
+  <si>
+    <t>Code/Design</t>
+  </si>
+  <si>
+    <t>Build Invoice GUI</t>
+  </si>
+  <si>
+    <t>5:32PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug GUI </t>
   </si>
 </sst>
 </file>
@@ -767,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H64"/>
+  <dimension ref="A3:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,11 +1576,45 @@
       <c r="B64" t="s">
         <v>121</v>
       </c>
+      <c r="C64" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="F64" t="s">
         <v>110</v>
       </c>
       <c r="G64" t="s">
         <v>123</v>
+      </c>
+      <c r="H64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="4">
+        <v>0.19027777777777777</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E65">
+        <v>58</v>
+      </c>
+      <c r="F65" t="s">
+        <v>126</v>
+      </c>
+      <c r="G65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>128</v>
+      </c>
+      <c r="F66" t="s">
+        <v>108</v>
+      </c>
+      <c r="G66" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Invoice GUI now correctly searches client names and displays. Now need to display client orders
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63486BA-ECB5-497C-BD59-8B9909EFB79D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21A30A0-59C7-4CF9-8DD2-A3130C56674E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -414,7 +414,7 @@
     <t>5:32PM</t>
   </si>
   <si>
-    <t xml:space="preserve">Debug GUI </t>
+    <t xml:space="preserve">Coding functionality for the new invoice page </t>
   </si>
 </sst>
 </file>
@@ -788,7 +788,7 @@
   <dimension ref="A3:H66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1611,7 @@
         <v>128</v>
       </c>
       <c r="F66" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G66" t="s">
         <v>129</v>

</xml_diff>

<commit_message>
newInvoiceCandS (create and search) now successfully shows in GUI. Next is coding the orders to show up and their details to show on doubleclick
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21A30A0-59C7-4CF9-8DD2-A3130C56674E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1526823-5E98-42F2-8587-32C1D78191F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19185" yWindow="-3615" windowWidth="16200" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="139">
   <si>
     <t>Delta</t>
   </si>
@@ -414,7 +414,34 @@
     <t>5:32PM</t>
   </si>
   <si>
-    <t xml:space="preserve">Coding functionality for the new invoice page </t>
+    <t>4:42PM</t>
+  </si>
+  <si>
+    <t>Build simpler invoice gui =&gt; for time's sake</t>
+  </si>
+  <si>
+    <t>Only allow a single invoice to be selected from all unpaid invoices, instead of sending an invoice w/ ability to batch orders together</t>
+  </si>
+  <si>
+    <t>Create GUI</t>
+  </si>
+  <si>
+    <t>4:56PM</t>
+  </si>
+  <si>
+    <t>Create GUI in Qt Designer</t>
+  </si>
+  <si>
+    <t>now need to import to program code</t>
+  </si>
+  <si>
+    <t>4:57PM</t>
+  </si>
+  <si>
+    <t>5:09PM</t>
+  </si>
+  <si>
+    <t>Debug GUI for newInvoiceCandS not showing correctly</t>
   </si>
 </sst>
 </file>
@@ -785,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H66"/>
+  <dimension ref="A3:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,7 +1616,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" s="4">
         <v>0.19027777777777777</v>
       </c>
@@ -1606,15 +1633,56 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>43810</v>
+      </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E66">
+        <v>14</v>
       </c>
       <c r="F66" t="s">
+        <v>132</v>
+      </c>
+      <c r="G66" t="s">
+        <v>134</v>
+      </c>
+      <c r="H66" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F67" t="s">
         <v>110</v>
       </c>
-      <c r="G66" t="s">
-        <v>129</v>
+      <c r="G67" t="s">
+        <v>130</v>
+      </c>
+      <c r="H67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F68" t="s">
+        <v>108</v>
+      </c>
+      <c r="G68" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setting up newInvoiceCandS page functionality
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1526823-5E98-42F2-8587-32C1D78191F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDD492-26D4-4177-A563-49107A924CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
   <si>
     <t>Delta</t>
   </si>
@@ -442,6 +442,15 @@
   </si>
   <si>
     <t>Debug GUI for newInvoiceCandS not showing correctly</t>
+  </si>
+  <si>
+    <t>5:12PM</t>
+  </si>
+  <si>
+    <t>Quick fix. 2 variables not named correctly</t>
+  </si>
+  <si>
+    <t>Setting up code for newInvoiceCandS page functionality</t>
   </si>
 </sst>
 </file>
@@ -812,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H68"/>
+  <dimension ref="A3:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,11 +1687,31 @@
       <c r="B68" s="4" t="s">
         <v>137</v>
       </c>
+      <c r="C68" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="F68" t="s">
         <v>108</v>
       </c>
       <c r="G68" t="s">
         <v>138</v>
+      </c>
+      <c r="H68" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="4">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="F69" t="s">
+        <v>110</v>
+      </c>
+      <c r="G69" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
newInvoice_orderList shows correctly, and is also now in correct format for MVC. Will follow this format from now on. Will change other formats if have the time
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DDD492-26D4-4177-A563-49107A924CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A47D29-747F-49C4-AF55-A484F1DF536F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="144">
   <si>
     <t>Delta</t>
   </si>
@@ -451,6 +451,12 @@
   </si>
   <si>
     <t>Setting up code for newInvoiceCandS page functionality</t>
+  </si>
+  <si>
+    <t>7:38PM</t>
+  </si>
+  <si>
+    <t>Slow Code</t>
   </si>
 </sst>
 </file>
@@ -821,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H69"/>
+  <dimension ref="A3:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,6 +1720,14 @@
         <v>141</v>
       </c>
     </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>142</v>
+      </c>
+      <c r="F70" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
products now show up on newInvoiceCandS page.
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A47D29-747F-49C4-AF55-A484F1DF536F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A29B58-B52C-4ED6-885A-84ED46140396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="150">
   <si>
     <t>Delta</t>
   </si>
@@ -457,6 +457,24 @@
   </si>
   <si>
     <t>Slow Code</t>
+  </si>
+  <si>
+    <t>9:34PM</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Got newInvoiceCandS gui almost all working</t>
+  </si>
+  <si>
+    <t>11:40AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding products to show up on newInvoiceCandS, and then beginning to code the mailto: </t>
+  </si>
+  <si>
+    <t>GUI now correctly shows all products through a convoluted SQLite3 query. Much time taken to build the query into 1 call</t>
   </si>
 </sst>
 </file>
@@ -827,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H70"/>
+  <dimension ref="A3:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,8 +1742,43 @@
       <c r="B70" t="s">
         <v>142</v>
       </c>
+      <c r="C70" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E70" t="s">
+        <v>145</v>
+      </c>
       <c r="F70" t="s">
         <v>143</v>
+      </c>
+      <c r="G70" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>43811</v>
+      </c>
+      <c r="B72" t="s">
+        <v>147</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>68</v>
+      </c>
+      <c r="F72" t="s">
+        <v>110</v>
+      </c>
+      <c r="G72" t="s">
+        <v>148</v>
+      </c>
+      <c r="H72" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enabled high dpi scaling for computers that do not have the standard sizes for apps or text
</commit_message>
<xml_diff>
--- a/ProjectFiles/082819-CIS598_LogBook.xlsx
+++ b/ProjectFiles/082819-CIS598_LogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\PycharmProjects\InvApp\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A29B58-B52C-4ED6-885A-84ED46140396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2246D36A-BB07-4C7E-9FAD-B84C7E0B7E1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19620" xr2:uid="{3F57D059-072D-48BA-A9B8-491AD0D49EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="152">
   <si>
     <t>Delta</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>GUI now correctly shows all products through a convoluted SQLite3 query. Much time taken to build the query into 1 call</t>
+  </si>
+  <si>
+    <t>2:48PM</t>
+  </si>
+  <si>
+    <t>Trying to find ways to size fonts correctly. If WindowsOS app size = 100% and font size = 100%, everything looks fine. Only when these values change do label fonts get sized incorrectly</t>
   </si>
 </sst>
 </file>
@@ -845,24 +851,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231EEA9-35CB-4E5F-8BA7-67BB9CC135E7}">
-  <dimension ref="A3:H72"/>
+  <dimension ref="A3:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.26953125" customWidth="1"/>
     <col min="7" max="7" width="111" customWidth="1"/>
-    <col min="8" max="8" width="90.42578125" customWidth="1"/>
+    <col min="8" max="8" width="90.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>38</v>
       </c>
@@ -870,8 +876,8 @@
         <v>101419</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -897,7 +903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>43705</v>
       </c>
@@ -923,7 +929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>43705</v>
       </c>
@@ -949,7 +955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>43726</v>
       </c>
@@ -972,7 +978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -992,7 +998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>43745</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>43747</v>
       </c>
@@ -1035,7 +1041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1052,7 +1058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>43749</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>43752</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>43756</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>43769</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>43770</v>
       </c>
@@ -1178,7 +1184,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>43773</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>43776</v>
       </c>
@@ -1224,7 +1230,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>56</v>
       </c>
@@ -1241,7 +1247,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>43777</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>63</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>43782</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>43784</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>43788</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B43" s="4" t="s">
         <v>76</v>
       </c>
@@ -1370,7 +1376,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>43789</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>81</v>
       </c>
@@ -1404,7 +1410,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>82</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>43791</v>
       </c>
@@ -1435,7 +1441,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>43795</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>43796</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>73</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>43808</v>
       </c>
@@ -1521,7 +1527,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>43809</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>87</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B60" s="4">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B61" s="4">
         <v>9.5138888888888884E-2</v>
       </c>
@@ -1595,7 +1601,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>113</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>118</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>121</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B65" s="4">
         <v>0.19027777777777777</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>43810</v>
       </c>
@@ -1689,7 +1695,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" t="s">
         <v>136</v>
@@ -1707,7 +1713,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B68" s="4" t="s">
         <v>137</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>139</v>
       </c>
@@ -1738,7 +1744,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>142</v>
       </c>
@@ -1755,7 +1761,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>43811</v>
       </c>
@@ -1779,6 +1785,20 @@
       </c>
       <c r="H72" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="2">
+        <v>43812</v>
+      </c>
+      <c r="B73" t="s">
+        <v>150</v>
+      </c>
+      <c r="F73" t="s">
+        <v>110</v>
+      </c>
+      <c r="G73" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>